<commit_message>
Update ExcelData model and add SignalR functionality
</commit_message>
<xml_diff>
--- a/FPT_Vote/Sample.xlsx
+++ b/FPT_Vote/Sample.xlsx
@@ -12,7 +12,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+  <si>
+    <t xml:space="preserve">Id</t>
+  </si>
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -96,37 +99,49 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>3</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
         <v>100</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>5</v>
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
         <v>150</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>7</v>
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
         <v>120</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update binary files and code in FPT_Vote project
</commit_message>
<xml_diff>
--- a/FPT_Vote/Sample.xlsx
+++ b/FPT_Vote/Sample.xlsx
@@ -6,13 +6,14 @@
     <workbookView tabRatio="600"/>
   </bookViews>
   <sheets>
-    <sheet name="SampleSheet" sheetId="1" r:id="rId3"/>
+    <sheet name="SampleSheet_1" sheetId="1" r:id="rId3"/>
+    <sheet name="SampleSheet_2" sheetId="2" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -60,6 +61,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group Name</t>
   </si>
 </sst>
 </file>
@@ -267,4 +271,50 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>